<commit_message>
SET up note, and BE
</commit_message>
<xml_diff>
--- a/Ke_hoach_DACNTT2-final.xlsx
+++ b/Ke_hoach_DACNTT2-final.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DACNNT2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DACNNT2\DACNTT2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B6295E9-7453-4088-867A-94FD34264A2E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17DAC8B1-FC2E-4790-AA9F-2C264DE3CF9E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11712" windowHeight="4500" xr2:uid="{469F8995-603E-4579-9AE9-0AB647CF7390}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="49">
   <si>
     <t>XÁC NHẬN CỦA GIẢNG VIÊN HƯỚNG DẪN</t>
   </si>
@@ -254,6 +254,16 @@
     <t>FE cho user:
 -Trang quản lý tài khoản để user có option đăng nhập để lưu các bài viết, hoặc xem lại các bài đã đọc gần đây.
 Fetch dữ liệu lên FE</t>
+  </si>
+  <si>
+    <t>-Dữ liệu sẽ lấy xuống trong 7 trang báo đã note trong repo của dự án.
+-Các thông tin lưu vào DB bao gồm URL, E16ảnh bài báo, Tiêu đề bài báo, ngày post bài báo.
+-Công nghệ sử dụng MERN
+-Link repo dữ án: https://github.com/Cuong15061999/DACNTT2</t>
+  </si>
+  <si>
+    <t>-Công nghệ sử dụng crawl Dữ liệu RSS or Cherio
+ -….</t>
   </si>
 </sst>
 </file>
@@ -452,7 +462,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
@@ -490,12 +500,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="6" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -514,6 +518,15 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -533,17 +546,17 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -865,8 +878,8 @@
   </sheetPr>
   <dimension ref="A1:AA33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" topLeftCell="D15" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -882,15 +895,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
@@ -913,15 +926,15 @@
       <c r="AA1" s="1"/>
     </row>
     <row r="2" spans="1:27" ht="26.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
@@ -977,11 +990,11 @@
       <c r="B4" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="30" t="s">
+      <c r="C4" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
@@ -1008,10 +1021,10 @@
     <row r="5" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="4"/>
-      <c r="C5" s="31" t="s">
+      <c r="C5" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="29"/>
+      <c r="D5" s="30"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
@@ -1072,10 +1085,10 @@
     <row r="7" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="4"/>
-      <c r="C7" s="31" t="s">
+      <c r="C7" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="29"/>
+      <c r="D7" s="30"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
@@ -1138,10 +1151,10 @@
       <c r="B9" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="30" t="s">
+      <c r="C9" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="29"/>
+      <c r="D9" s="30"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -1209,7 +1222,7 @@
       <c r="C11" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="20" t="s">
+      <c r="D11" s="18" t="s">
         <v>29</v>
       </c>
       <c r="E11" s="1"/>
@@ -1390,10 +1403,10 @@
       <c r="E16" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="F16" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="G16" s="15" t="s">
+      <c r="F16" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="G16" s="33" t="s">
         <v>4</v>
       </c>
       <c r="H16" s="1"/>
@@ -1432,13 +1445,13 @@
         <f t="shared" ref="D17:D31" si="1">C17+6</f>
         <v>44871</v>
       </c>
-      <c r="E17" s="22" t="s">
+      <c r="E17" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="F17" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="G17" s="15" t="s">
+      <c r="F17" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="G17" s="33" t="s">
         <v>4</v>
       </c>
       <c r="H17" s="1"/>
@@ -1473,17 +1486,17 @@
         <f t="shared" si="0"/>
         <v>44872</v>
       </c>
-      <c r="D18" s="21">
+      <c r="D18" s="19">
         <f t="shared" si="1"/>
         <v>44878</v>
       </c>
-      <c r="E18" s="34" t="s">
+      <c r="E18" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="F18" s="15" t="s">
+      <c r="F18" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="G18" s="15" t="s">
+      <c r="G18" s="33" t="s">
         <v>4</v>
       </c>
       <c r="H18" s="1"/>
@@ -1522,13 +1535,13 @@
         <f t="shared" si="1"/>
         <v>44885</v>
       </c>
-      <c r="E19" s="33" t="s">
+      <c r="E19" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="F19" s="15" t="s">
+      <c r="F19" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="G19" s="15" t="s">
+      <c r="G19" s="33" t="s">
         <v>4</v>
       </c>
       <c r="H19" s="1"/>
@@ -1570,10 +1583,10 @@
       <c r="E20" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="F20" s="15" t="s">
+      <c r="F20" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="G20" s="15" t="s">
+      <c r="G20" s="33" t="s">
         <v>4</v>
       </c>
       <c r="H20" s="1"/>
@@ -1615,10 +1628,10 @@
       <c r="E21" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="F21" s="15" t="s">
+      <c r="F21" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="G21" s="15" t="s">
+      <c r="G21" s="33" t="s">
         <v>4</v>
       </c>
       <c r="H21" s="1"/>
@@ -1649,19 +1662,19 @@
       <c r="B22" s="10">
         <v>17</v>
       </c>
-      <c r="C22" s="17">
+      <c r="C22" s="15">
         <f t="shared" si="0"/>
         <v>44900</v>
       </c>
-      <c r="D22" s="17">
+      <c r="D22" s="15">
         <f t="shared" si="1"/>
         <v>44906</v>
       </c>
-      <c r="E22" s="32" t="s">
+      <c r="E22" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="F22" s="26"/>
-      <c r="G22" s="27"/>
+      <c r="F22" s="34"/>
+      <c r="G22" s="35"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
@@ -1698,13 +1711,13 @@
         <f t="shared" si="1"/>
         <v>44913</v>
       </c>
-      <c r="E23" s="22" t="s">
+      <c r="E23" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="F23" s="15" t="s">
+      <c r="F23" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="G23" s="15" t="s">
+      <c r="G23" s="33" t="s">
         <v>4</v>
       </c>
       <c r="H23" s="1"/>
@@ -1739,17 +1752,17 @@
         <f t="shared" si="0"/>
         <v>44914</v>
       </c>
-      <c r="D24" s="21">
+      <c r="D24" s="19">
         <f t="shared" si="1"/>
         <v>44920</v>
       </c>
-      <c r="E24" s="35" t="s">
+      <c r="E24" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="F24" s="15" t="s">
+      <c r="F24" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="G24" s="15" t="s">
+      <c r="G24" s="33" t="s">
         <v>4</v>
       </c>
       <c r="H24" s="1"/>
@@ -1784,17 +1797,17 @@
         <f t="shared" si="0"/>
         <v>44921</v>
       </c>
-      <c r="D25" s="21">
+      <c r="D25" s="19">
         <f t="shared" si="1"/>
         <v>44927</v>
       </c>
-      <c r="E25" s="35" t="s">
+      <c r="E25" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="F25" s="15" t="s">
+      <c r="F25" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="G25" s="15" t="s">
+      <c r="G25" s="33" t="s">
         <v>4</v>
       </c>
       <c r="H25" s="1"/>
@@ -1829,17 +1842,17 @@
         <f t="shared" si="0"/>
         <v>44928</v>
       </c>
-      <c r="D26" s="21">
+      <c r="D26" s="19">
         <f t="shared" si="1"/>
         <v>44934</v>
       </c>
-      <c r="E26" s="35" t="s">
+      <c r="E26" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="F26" s="15" t="s">
+      <c r="F26" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="G26" s="15" t="s">
+      <c r="G26" s="33" t="s">
         <v>4</v>
       </c>
       <c r="H26" s="1"/>
@@ -1874,17 +1887,17 @@
         <f t="shared" si="0"/>
         <v>44935</v>
       </c>
-      <c r="D27" s="21">
+      <c r="D27" s="19">
         <f t="shared" si="1"/>
         <v>44941</v>
       </c>
-      <c r="E27" s="23" t="s">
+      <c r="E27" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="F27" s="15" t="s">
+      <c r="F27" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="G27" s="15" t="s">
+      <c r="G27" s="33" t="s">
         <v>4</v>
       </c>
       <c r="H27" s="1"/>
@@ -1923,13 +1936,13 @@
         <f t="shared" si="1"/>
         <v>44948</v>
       </c>
-      <c r="E28" s="16" t="s">
+      <c r="E28" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="F28" s="15" t="s">
+      <c r="F28" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="G28" s="15" t="s">
+      <c r="G28" s="33" t="s">
         <v>4</v>
       </c>
       <c r="H28" s="1"/>
@@ -1953,7 +1966,7 @@
       <c r="Z28" s="1"/>
       <c r="AA28" s="1"/>
     </row>
-    <row r="29" spans="1:27" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:27" ht="33.6" x14ac:dyDescent="0.3">
       <c r="A29" s="11">
         <v>14</v>
       </c>
@@ -1968,13 +1981,13 @@
         <f t="shared" si="1"/>
         <v>44955</v>
       </c>
-      <c r="E29" s="16" t="s">
+      <c r="E29" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="F29" s="15" t="s">
+      <c r="F29" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="G29" s="15" t="s">
+      <c r="G29" s="33" t="s">
         <v>4</v>
       </c>
       <c r="H29" s="1"/>
@@ -2005,19 +2018,19 @@
       <c r="B30" s="10">
         <v>25</v>
       </c>
-      <c r="C30" s="17">
+      <c r="C30" s="15">
         <f t="shared" si="0"/>
         <v>44956</v>
       </c>
-      <c r="D30" s="17">
+      <c r="D30" s="15">
         <f t="shared" si="1"/>
         <v>44962</v>
       </c>
-      <c r="E30" s="25" t="s">
+      <c r="E30" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="F30" s="26"/>
-      <c r="G30" s="27"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="28"/>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
@@ -2046,19 +2059,19 @@
       <c r="B31" s="10">
         <v>26</v>
       </c>
-      <c r="C31" s="17">
+      <c r="C31" s="15">
         <f t="shared" si="0"/>
         <v>44963</v>
       </c>
-      <c r="D31" s="17">
+      <c r="D31" s="15">
         <f t="shared" si="1"/>
         <v>44969</v>
       </c>
-      <c r="E31" s="25" t="s">
+      <c r="E31" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="F31" s="26"/>
-      <c r="G31" s="27"/>
+      <c r="F31" s="27"/>
+      <c r="G31" s="28"/>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
@@ -2112,12 +2125,12 @@
     <row r="33" spans="1:27" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
-      <c r="C33" s="18" t="s">
+      <c r="C33" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="D33" s="19"/>
-      <c r="E33" s="19"/>
-      <c r="F33" s="18" t="s">
+      <c r="D33" s="17"/>
+      <c r="E33" s="17"/>
+      <c r="F33" s="16" t="s">
         <v>0</v>
       </c>
       <c r="G33" s="1"/>

</xml_diff>